<commit_message>
Gurukrip SHG Audit docs
</commit_message>
<xml_diff>
--- a/src/assets/docs/gurukripa_shg/Ferbuary-2024/ഗുരുകൃപ SHG - ഓഡിറ്റ്-February-18-2024.xlsx
+++ b/src/assets/docs/gurukripa_shg/Ferbuary-2024/ഗുരുകൃപ SHG - ഓഡിറ്റ്-February-18-2024.xlsx
@@ -134,12 +134,6 @@
     <t xml:space="preserve">പുറം പലിശ(10K) </t>
   </si>
   <si>
-    <t xml:space="preserve">പുറം വായ്പ (INTEREST 3%) </t>
-  </si>
-  <si>
-    <t>പുറം പലിശ (INTEREST 3%)</t>
-  </si>
-  <si>
     <t>HOSPITAL EMERGENCY</t>
   </si>
   <si>
@@ -185,7 +179,13 @@
     <t xml:space="preserve">ഓണം അഡ്വാൻസ് </t>
   </si>
   <si>
-    <t>ലോൺ അഡ്ജസ്റ്മെന്റ്സ്  (Old Bank Withdrawal)</t>
+    <t>ലോൺ അഡ്ജസ്റ്മെന്റ്സ്  (IDCB Loan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ബിസിനസ്സ്  വായ്പ (ROI 3%) </t>
+  </si>
+  <si>
+    <t>ബിസിനസ്സ്  പലിശ (ROI 3%)</t>
   </si>
 </sst>
 </file>
@@ -606,42 +606,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -654,6 +618,42 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -997,35 +997,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
       <c r="Q1" s="10">
         <v>45338</v>
       </c>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="51"/>
+      <c r="C2" s="56"/>
       <c r="N2" s="26"/>
     </row>
     <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="I3" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="54"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="I3" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="59"/>
       <c r="M3" s="31"/>
       <c r="N3" s="31"/>
       <c r="O3" s="31"/>
@@ -1084,7 +1084,7 @@
         <v>18</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="S5" s="17" t="s">
         <v>9</v>
@@ -1130,7 +1130,7 @@
       <c r="N6" s="27">
         <v>900</v>
       </c>
-      <c r="O6" s="62">
+      <c r="O6" s="50">
         <v>0</v>
       </c>
       <c r="P6" s="28"/>
@@ -1187,7 +1187,7 @@
       <c r="N7" s="27">
         <v>200</v>
       </c>
-      <c r="O7" s="62">
+      <c r="O7" s="50">
         <v>0</v>
       </c>
       <c r="P7" s="28"/>
@@ -1244,7 +1244,7 @@
       <c r="N8" s="27">
         <v>1100</v>
       </c>
-      <c r="O8" s="62">
+      <c r="O8" s="50">
         <v>1100</v>
       </c>
       <c r="P8" s="28"/>
@@ -1301,7 +1301,7 @@
       <c r="N9" s="27">
         <v>200</v>
       </c>
-      <c r="O9" s="62">
+      <c r="O9" s="50">
         <v>0</v>
       </c>
       <c r="P9" s="28"/>
@@ -1358,7 +1358,7 @@
       <c r="N10" s="27">
         <v>0</v>
       </c>
-      <c r="O10" s="62">
+      <c r="O10" s="50">
         <v>0</v>
       </c>
       <c r="P10" s="28"/>
@@ -1415,7 +1415,7 @@
       <c r="N11" s="27">
         <v>600</v>
       </c>
-      <c r="O11" s="62">
+      <c r="O11" s="50">
         <v>400</v>
       </c>
       <c r="P11" s="28"/>
@@ -1472,7 +1472,7 @@
       <c r="N12" s="27">
         <v>0</v>
       </c>
-      <c r="O12" s="62">
+      <c r="O12" s="50">
         <v>0</v>
       </c>
       <c r="P12" s="28"/>
@@ -1529,7 +1529,7 @@
       <c r="N13" s="27">
         <v>0</v>
       </c>
-      <c r="O13" s="62">
+      <c r="O13" s="50">
         <v>200</v>
       </c>
       <c r="P13" s="28"/>
@@ -1586,7 +1586,7 @@
       <c r="N14" s="27">
         <v>400</v>
       </c>
-      <c r="O14" s="62">
+      <c r="O14" s="50">
         <v>0</v>
       </c>
       <c r="P14" s="28"/>
@@ -1643,7 +1643,7 @@
       <c r="N15" s="27">
         <v>400</v>
       </c>
-      <c r="O15" s="62">
+      <c r="O15" s="50">
         <v>400</v>
       </c>
       <c r="P15" s="28"/>
@@ -1700,7 +1700,7 @@
       <c r="N16" s="27">
         <v>0</v>
       </c>
-      <c r="O16" s="62">
+      <c r="O16" s="50">
         <v>200</v>
       </c>
       <c r="P16" s="28"/>
@@ -1757,7 +1757,7 @@
       <c r="N17" s="27">
         <v>600</v>
       </c>
-      <c r="O17" s="62">
+      <c r="O17" s="50">
         <v>0</v>
       </c>
       <c r="P17" s="28"/>
@@ -1814,7 +1814,7 @@
       <c r="N18" s="27">
         <v>200</v>
       </c>
-      <c r="O18" s="62">
+      <c r="O18" s="50">
         <v>800</v>
       </c>
       <c r="P18" s="28"/>
@@ -1871,7 +1871,7 @@
       <c r="N19" s="27">
         <v>800</v>
       </c>
-      <c r="O19" s="62">
+      <c r="O19" s="50">
         <v>400</v>
       </c>
       <c r="P19" s="28"/>
@@ -2062,25 +2062,25 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
       <c r="P1" s="10">
         <v>45338</v>
       </c>
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="56"/>
+      <c r="B2" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="61"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -2095,22 +2095,22 @@
       <c r="Q2" s="7"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
+      <c r="I3" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
       <c r="P3" s="19">
         <v>550</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>50</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
@@ -2830,25 +2830,25 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
       <c r="P1" s="10">
         <v>45338</v>
       </c>
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="51"/>
+      <c r="B2" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="56"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -2863,22 +2863,22 @@
       <c r="Q2" s="7"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
+      <c r="I3" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
       <c r="P3" s="19">
         <v>550</v>
       </c>
@@ -3585,7 +3585,7 @@
   </sheetPr>
   <dimension ref="B2:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -3595,9 +3595,9 @@
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" style="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="7" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" style="51" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="7" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" style="7" customWidth="1"/>
@@ -3607,26 +3607,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="62"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="E3" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="57"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="E3" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="K3" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="59"/>
-      <c r="M3" s="60"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="K3" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="64"/>
+      <c r="M3" s="65"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D4" s="7"/>
@@ -3650,31 +3650,31 @@
         <v>25</v>
       </c>
       <c r="G5" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="24" t="s">
         <v>26</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="24" t="s">
-        <v>28</v>
       </c>
       <c r="N5" s="18" t="s">
         <v>24</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:15" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -3702,7 +3702,7 @@
       <c r="H6" s="34">
         <v>1200</v>
       </c>
-      <c r="I6" s="64">
+      <c r="I6" s="52">
         <v>622</v>
       </c>
       <c r="J6" s="37">
@@ -3738,7 +3738,7 @@
       </c>
       <c r="G7" s="37"/>
       <c r="H7" s="34"/>
-      <c r="I7" s="64">
+      <c r="I7" s="52">
         <v>622</v>
       </c>
       <c r="J7" s="37">
@@ -3778,18 +3778,16 @@
       <c r="H8" s="34">
         <v>2700</v>
       </c>
-      <c r="I8" s="64">
+      <c r="I8" s="52">
         <v>622</v>
       </c>
-      <c r="J8" s="37">
-        <v>1000</v>
-      </c>
+      <c r="J8" s="37"/>
       <c r="K8" s="37"/>
       <c r="L8" s="37"/>
       <c r="M8" s="41"/>
       <c r="N8" s="33">
         <f t="shared" si="0"/>
-        <v>14722</v>
+        <v>13722</v>
       </c>
       <c r="O8" s="38"/>
     </row>
@@ -3816,7 +3814,7 @@
         <v>10000</v>
       </c>
       <c r="H9" s="34">
-        <v>900</v>
+        <v>1950</v>
       </c>
       <c r="I9" s="37">
         <v>622</v>
@@ -3835,7 +3833,7 @@
       </c>
       <c r="N9" s="33">
         <f t="shared" si="0"/>
-        <v>24672</v>
+        <v>25722</v>
       </c>
       <c r="O9" s="38"/>
     </row>
@@ -3864,7 +3862,7 @@
       <c r="H10" s="34">
         <v>1200</v>
       </c>
-      <c r="I10" s="64">
+      <c r="I10" s="52">
         <v>622</v>
       </c>
       <c r="J10" s="37">
@@ -3898,24 +3896,18 @@
         <f>'പലിശ(10k)'!Q11</f>
         <v>50</v>
       </c>
-      <c r="G11" s="37">
-        <v>10000</v>
-      </c>
-      <c r="H11" s="34">
-        <v>2300</v>
-      </c>
-      <c r="I11" s="64">
+      <c r="G11" s="37"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="52">
         <v>622</v>
       </c>
-      <c r="J11" s="37">
-        <v>0</v>
-      </c>
+      <c r="J11" s="37"/>
       <c r="K11" s="37"/>
       <c r="L11" s="37"/>
       <c r="M11" s="41"/>
       <c r="N11" s="33">
         <f t="shared" si="0"/>
-        <v>13022</v>
+        <v>722</v>
       </c>
       <c r="O11" s="38"/>
     </row>
@@ -3942,9 +3934,9 @@
         <v>5000</v>
       </c>
       <c r="H12" s="34">
-        <v>1250</v>
-      </c>
-      <c r="I12" s="64">
+        <v>1050</v>
+      </c>
+      <c r="I12" s="52">
         <v>622</v>
       </c>
       <c r="J12" s="37">
@@ -3955,7 +3947,7 @@
       <c r="M12" s="41"/>
       <c r="N12" s="33">
         <f t="shared" si="0"/>
-        <v>14772</v>
+        <v>14572</v>
       </c>
       <c r="O12" s="38"/>
     </row>
@@ -3990,16 +3982,14 @@
       <c r="J13" s="37">
         <v>1000</v>
       </c>
-      <c r="K13" s="37">
-        <v>500</v>
-      </c>
+      <c r="K13" s="37"/>
       <c r="L13" s="40">
         <v>200</v>
       </c>
       <c r="M13" s="41"/>
       <c r="N13" s="33">
         <f t="shared" si="0"/>
-        <v>17972</v>
+        <v>17472</v>
       </c>
       <c r="O13" s="38"/>
     </row>
@@ -4027,9 +4017,7 @@
       <c r="I14" s="37">
         <v>622</v>
       </c>
-      <c r="J14" s="37">
-        <v>0</v>
-      </c>
+      <c r="J14" s="37"/>
       <c r="K14" s="37"/>
       <c r="L14" s="37"/>
       <c r="M14" s="41">
@@ -4062,7 +4050,7 @@
       </c>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
-      <c r="I15" s="64">
+      <c r="I15" s="52">
         <v>0</v>
       </c>
       <c r="J15" s="37">
@@ -4077,7 +4065,7 @@
       </c>
       <c r="O15" s="38"/>
     </row>
-    <row r="16" spans="2:15" s="66" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" s="54" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34">
         <v>11</v>
       </c>
@@ -4121,7 +4109,7 @@
         <f t="shared" si="0"/>
         <v>27322</v>
       </c>
-      <c r="O16" s="65"/>
+      <c r="O16" s="53"/>
     </row>
     <row r="17" spans="2:15" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="34">
@@ -4146,20 +4134,18 @@
         <v>5000</v>
       </c>
       <c r="H17" s="34">
-        <v>450</v>
-      </c>
-      <c r="I17" s="64">
+        <v>1050</v>
+      </c>
+      <c r="I17" s="52">
         <v>622</v>
       </c>
-      <c r="J17" s="34">
-        <v>0</v>
-      </c>
+      <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
       <c r="M17" s="41"/>
       <c r="N17" s="33">
         <f t="shared" si="0"/>
-        <v>8572</v>
+        <v>9172</v>
       </c>
       <c r="O17" s="38"/>
     </row>
@@ -4186,9 +4172,9 @@
         <v>5000</v>
       </c>
       <c r="H18" s="34">
-        <v>900</v>
-      </c>
-      <c r="I18" s="64">
+        <v>1200</v>
+      </c>
+      <c r="I18" s="52">
         <v>622</v>
       </c>
       <c r="J18" s="34">
@@ -4199,7 +4185,7 @@
       <c r="M18" s="41"/>
       <c r="N18" s="33">
         <f t="shared" si="0"/>
-        <v>7622</v>
+        <v>7922</v>
       </c>
       <c r="O18" s="38"/>
     </row>
@@ -4226,20 +4212,18 @@
         <v>10000</v>
       </c>
       <c r="H19" s="34">
-        <v>1200</v>
-      </c>
-      <c r="I19" s="64">
+        <v>900</v>
+      </c>
+      <c r="I19" s="52">
         <v>622</v>
       </c>
-      <c r="J19" s="34">
-        <v>0</v>
-      </c>
+      <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="34"/>
       <c r="M19" s="41"/>
       <c r="N19" s="33">
         <f>SUM(D19:M19)</f>
-        <v>12122</v>
+        <v>11822</v>
       </c>
       <c r="O19" s="38"/>
     </row>
@@ -4266,11 +4250,11 @@
       </c>
       <c r="G21" s="34">
         <f>SUM(G6:G19)</f>
-        <v>90000</v>
+        <v>80000</v>
       </c>
       <c r="H21" s="34">
         <f>SUM(H6:H20)</f>
-        <v>17200</v>
+        <v>16350</v>
       </c>
       <c r="I21" s="34">
         <f>SUM(I2:I20)</f>
@@ -4278,11 +4262,11 @@
       </c>
       <c r="J21" s="34">
         <f>SUM(J6:J20)</f>
-        <v>10000</v>
+        <v>9000</v>
       </c>
       <c r="K21" s="34">
         <f>SUM(K6:K19)</f>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="L21" s="34">
         <f>SUM(L6:L19)</f>
@@ -4294,7 +4278,7 @@
       </c>
       <c r="N21" s="43">
         <f>SUM(N6:N20)</f>
-        <v>195436</v>
+        <v>183086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>